<commit_message>
Time-varying expeirments in 2d
these experiments are working and are producing valid bounds.
</commit_message>
<xml_diff>
--- a/experiments/peak_delay_experiments_report.xlsx
+++ b/experiments/peak_delay_experiments_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\Documents\MATLAB\time_delay\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2034761-9FDA-4A37-8485-9F22C41C9795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705B55FD-84A4-42B9-AF7C-E3B8167A30E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7680" yWindow="3240" windowWidth="23040" windowHeight="12195" xr2:uid="{BF636E8E-3835-4B7F-9C6E-1C26ABB38E2B}"/>
+    <workbookView xWindow="15615" yWindow="7740" windowWidth="23040" windowHeight="12195" xr2:uid="{BF636E8E-3835-4B7F-9C6E-1C26ABB38E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>order</t>
   </si>
@@ -47,7 +47,13 @@
     <t>Flow system: p(x) = -x_2</t>
   </si>
   <si>
-    <t>Twist system: p(x) = x_3</t>
+    <t>n=2</t>
+  </si>
+  <si>
+    <t>Time-var system: p(x) = x_2</t>
+  </si>
+  <si>
+    <t>Time-var system: p(x) = x_1</t>
   </si>
 </sst>
 </file>
@@ -402,15 +408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA22904A-C948-4D3A-AAF4-A7A08A840073}">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -456,12 +465,15 @@
         <v>-1.1727339538218899</v>
       </c>
       <c r="F4">
-        <v>1.1629537872309501</v>
+        <v>-1.1629537872309501</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -493,19 +505,75 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>1.20000000863969</v>
+        <v>1.2500000000698901</v>
       </c>
       <c r="C9">
-        <v>1.20000000863969</v>
+        <v>1.2500000053924201</v>
       </c>
       <c r="D9">
-        <v>1.20000000863969</v>
+        <v>0.95570317361146495</v>
+      </c>
+      <c r="E9">
+        <v>0.913761594166</v>
+      </c>
+      <c r="F9">
+        <v>0.91118772095365697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1.2500000047261901</v>
+      </c>
+      <c r="C13">
+        <v>1.2500000053924201</v>
+      </c>
+      <c r="D13">
+        <v>1.1978182268083599</v>
+      </c>
+      <c r="E13">
+        <v>0.854326158386573</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Continuation of time-var experiment
</commit_message>
<xml_diff>
--- a/experiments/peak_delay_experiments_report.xlsx
+++ b/experiments/peak_delay_experiments_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\Documents\MATLAB\time_delay\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705B55FD-84A4-42B9-AF7C-E3B8167A30E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C126D1C0-C946-48F0-892A-54AB2EDB7EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15615" yWindow="7740" windowWidth="23040" windowHeight="12195" xr2:uid="{BF636E8E-3835-4B7F-9C6E-1C26ABB38E2B}"/>
+    <workbookView xWindow="7680" yWindow="4485" windowWidth="23040" windowHeight="12195" xr2:uid="{BF636E8E-3835-4B7F-9C6E-1C26ABB38E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +567,9 @@
       </c>
       <c r="E13">
         <v>0.854326158386573</v>
+      </c>
+      <c r="F13">
+        <v>0.71826461805817998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>